<commit_message>
Changes for project structure
</commit_message>
<xml_diff>
--- a/src/test/java/com/inetbanking/testData/Data.xlsx
+++ b/src/test/java/com/inetbanking/testData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayanta\Desktop\project\iNETBanking_V1\src\test\java\com\inetbanking\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sayantabera/My_Work_Folder/Java_Projects/iNETBanking_V1/src/test/java/com/inetbanking/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01676930-BC94-4616-A395-331C984FE6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D55BA2-3ED4-A444-89B1-F19C8E6A7EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="500" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,15 +363,15 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,7 +379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -387,7 +387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -395,7 +395,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -403,7 +403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>

</xml_diff>